<commit_message>
update sample with url referencing a file
</commit_message>
<xml_diff>
--- a/sampledata/test_dataset_no_data.xlsx
+++ b/sampledata/test_dataset_no_data.xlsx
@@ -135,7 +135,7 @@
     <t>Dataset Data URL</t>
   </si>
   <si>
-    <t>http://lincs.hms.harvard.edu/</t>
+    <t>http://lincs.hms.harvard.edu/wordpress/wp-content/uploads/2015/02/CycIF_image_processing_09-21-2015.zip</t>
   </si>
   <si>
     <t>facility_batch_id</t>
@@ -179,7 +179,7 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -222,11 +222,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -270,7 +265,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -296,10 +291,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -323,13 +314,12 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="257" min="1" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="257" min="1" style="1" width="11.0714285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -494,7 +484,6 @@
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" display="jt@test.com"/>
     <hyperlink ref="B7" r:id="rId2" display="sallyt@test.com"/>
-    <hyperlink ref="B20" r:id="rId3" display="http://lincs.hms.harvard.edu/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -519,7 +508,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -568,12 +557,12 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="2" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>